<commit_message>
Added Updated sample script
Added updated sample script
</commit_message>
<xml_diff>
--- a/SampleScript/TestCase/DemoTest.xlsx
+++ b/SampleScript/TestCase/DemoTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>Run</t>
   </si>
@@ -51,16 +51,6 @@
     <t>click</t>
   </si>
   <si>
-    <t>参照フォルダ</t>
-    <rPh sb="0" eb="2">
-      <t>サンショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>E:\Open 2Test  c folder Back UP\New folder (3)\Xlsx_Testing\O2T_RegTest_Ph11\O2T_RegTest_Ph11</t>
-  </si>
-  <si>
     <t>wait</t>
   </si>
   <si>
@@ -70,21 +60,6 @@
     <t>textbox;TxtName</t>
   </si>
   <si>
-    <t>https://www.google.com</t>
-  </si>
-  <si>
-    <t>textbox;TxtSearch</t>
-  </si>
-  <si>
-    <t>button;BtnSearch</t>
-  </si>
-  <si>
-    <t>Set:open2test</t>
-  </si>
-  <si>
-    <t>link;linkO2t</t>
-  </si>
-  <si>
     <t>link;linkComments</t>
   </si>
   <si>
@@ -130,9 +105,6 @@
     <t>linktext:Comment</t>
   </si>
   <si>
-    <t>linktext:Welcome to Open2Test.org</t>
-  </si>
-  <si>
     <t>Launching the Website</t>
   </si>
   <si>
@@ -142,21 +114,6 @@
     <t>Applied wait for 100 m/s</t>
   </si>
   <si>
-    <t>Importing Test data file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setting text to search </t>
-  </si>
-  <si>
-    <t>Click on Button</t>
-  </si>
-  <si>
-    <t>Checking if given link is present</t>
-  </si>
-  <si>
-    <t>Click on link</t>
-  </si>
-  <si>
     <t>Checking link is present</t>
   </si>
   <si>
@@ -184,15 +141,36 @@
     <t>screencaptureoption</t>
   </si>
   <si>
-    <t>E:\AAVmwareDemo\
-TestData\Testdata.xlsx</t>
+    <t>E:\Open2Test\Open2Test_Selenium\SampleScript\TestData\Testdata.xlsx</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Importing Test data file. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Please traverse ==&gt; Open2Test_Selenium Downloaded folder ==&gt; Sample Script ==&gt; TestData ==&gt; TestData.xlsx
+ </t>
+    </r>
+  </si>
+  <si>
+    <t>http://www.open2test.org/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +194,17 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +220,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,11 +305,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -620,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -664,12 +657,12 @@
         <v>3</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -677,15 +670,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -701,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="11">
         <v>1000</v>
@@ -709,23 +702,23 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="4" t="s">
-        <v>39</v>
+      <c r="F6" s="15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -733,32 +726,32 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="11">
-        <v>1000</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
@@ -768,14 +761,14 @@
         <v>8</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -783,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="11">
         <v>1000</v>
@@ -797,17 +790,17 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -818,14 +811,14 @@
         <v>8</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -833,45 +826,53 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="11">
-        <v>1000</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="F13" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="11">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="F14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -879,17 +880,15 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C16" s="11">
+        <v>1000</v>
+      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -897,12 +896,14 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="11">
-        <v>1000</v>
-      </c>
-      <c r="D17" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="4"/>
     </row>
@@ -911,144 +912,78 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C18" s="11">
+        <v>1000</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30">
-      <c r="A21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30">
-      <c r="A22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="11">
-        <v>1000</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="11">
-        <v>1000</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
       <c r="C26" s="11"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1253,62 +1188,6 @@
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="4"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="4"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="4"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="4"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="4"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="4"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="4"/>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
@@ -1323,28 +1202,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="91.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1354,7 +1219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>